<commit_message>
refactor and added features
</commit_message>
<xml_diff>
--- a/Results/test.xlsx
+++ b/Results/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,107 +486,202 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>epochs_sedentairy_median_length</t>
+          <t>weight_median_sedentairy</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>alfa_sedentairy</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>sigma_sedentairy</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>gini_sedentairy</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>sedentairy_median_length</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>epochs_sedentairy_average_length</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>epochs_sedentairy_max_length</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>light_count</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>light_perc</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>epochs_light_perc</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>epochs_light_median_length</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>weight_median_light</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>alfa_light</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>sigma_light</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>gini_light</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>light_median_length</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>epochs_light_average_length</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>epochs_light_max_length</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>moderate_count</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>moderate_perc</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>epochs_moderate_perc</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>epochs_moderate_median_length</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>weight_median_moderate</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>alfa_moderate</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>sigma_moderate</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>gini_moderate</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>moderate_median_length</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>epochs_moderate_average_length</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>epochs_moderate_max_length</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>vigorous_count</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>vigorous_perc</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>epochs_vigorous_perc</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>epochs_vigorous_median_length</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>weight_median_vigorous</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>alfa_vigorous</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>sigma_vigorous</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>gini_vigorous</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>vigorous_median_length</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>epochs_vigorous_average_length</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>epochs_vigorous_max_length</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Sample_entropy</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>info_entropy</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>PLZC</t>
         </is>
       </c>
     </row>
@@ -597,94 +692,151 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>179625</v>
+        <v>179730</v>
       </c>
       <c r="C2" t="n">
-        <v>179625</v>
+        <v>179730</v>
       </c>
       <c r="D2" t="n">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E2" t="n">
-        <v>1.033333333333333</v>
+        <v>1.038</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5821465684815998</v>
+        <v>0.583</v>
       </c>
       <c r="G2" t="n">
-        <v>33.75</v>
+        <v>33.891</v>
       </c>
       <c r="H2" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" t="n">
-        <v>29.16666666666667</v>
+        <v>28.87</v>
       </c>
       <c r="J2" t="n">
-        <v>37.80487804878049</v>
+        <v>37.805</v>
       </c>
       <c r="K2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2.606</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.288</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.359</v>
+      </c>
+      <c r="O2" t="n">
         <v>2</v>
       </c>
-      <c r="L2" t="n">
-        <v>2.258064516129032</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="P2" t="n">
+        <v>2.226</v>
+      </c>
+      <c r="Q2" t="n">
         <v>6</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>125</v>
       </c>
-      <c r="O2" t="n">
-        <v>52.08333333333334</v>
-      </c>
-      <c r="P2" t="n">
-        <v>41.46341463414634</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>2</v>
-      </c>
-      <c r="R2" t="n">
-        <v>3.676470588235294</v>
-      </c>
       <c r="S2" t="n">
-        <v>16</v>
+        <v>52.301</v>
       </c>
       <c r="T2" t="n">
-        <v>12</v>
+        <v>41.463</v>
       </c>
       <c r="U2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="V2" t="n">
-        <v>12.19512195121951</v>
+        <v>2.175</v>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>0.202</v>
       </c>
       <c r="X2" t="n">
-        <v>1.2</v>
+        <v>0.509</v>
       </c>
       <c r="Y2" t="n">
         <v>2</v>
       </c>
       <c r="Z2" t="n">
+        <v>3.676</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>5.021</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>12.195</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>8.212999999999999</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>2.281</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL2" t="n">
         <v>33</v>
       </c>
-      <c r="AA2" t="n">
-        <v>13.75</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>8.536585365853659</v>
-      </c>
-      <c r="AC2" t="n">
+      <c r="AM2" t="n">
+        <v>13.808</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>8.537000000000001</v>
+      </c>
+      <c r="AO2" t="n">
         <v>5</v>
       </c>
-      <c r="AD2" t="n">
-        <v>4.714285714285714</v>
-      </c>
-      <c r="AE2" t="n">
+      <c r="AP2" t="n">
+        <v>1.672</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.254</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.313</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>4.714</v>
+      </c>
+      <c r="AU2" t="n">
         <v>7</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.507</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>5.375</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>